<commit_message>
Finished Excel Data Analysis Chapter 5
</commit_message>
<xml_diff>
--- a/LinkedIn/Excel_Data_Analysis/Exercise Files/Chapter05/MultipleCorrelations.xlsx
+++ b/LinkedIn/Excel_Data_Analysis/Exercise Files/Chapter05/MultipleCorrelations.xlsx
@@ -1,24 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21022"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Curtis\Desktop\Exercise Files\Chapter05\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rtalebiz\Desktop\Jupyter\Examples\LinkedIn\Excel_Data_Analysis\Exercise Files\Chapter05\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F5723E-B117-4D7A-B4B1-0347C4BF9E7A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80E656D9-9D51-4655-9A53-1F9EE4D775FB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2505" yWindow="2505" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -380,8 +386,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,6 +479,22 @@
       <c r="F5" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="G5">
+        <f>CORREL($A$2:$A$11, A2:A11)</f>
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ref="H5:J5" si="0">CORREL($A$2:$A$11, B2:B11)</f>
+        <v>-7.0616952177650114E-2</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>0.73719901064788396</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>0.48503173467607291</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -490,6 +512,22 @@
       <c r="F6" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="G6">
+        <f>CORREL($B$2:$B$11, A2:A11)</f>
+        <v>-7.0616952177650114E-2</v>
+      </c>
+      <c r="H6">
+        <f t="shared" ref="H6:J6" si="1">CORREL($B$2:$B$11, B2:B11)</f>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>-0.39911706248255019</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="1"/>
+        <v>0.20257937544884455</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -507,6 +545,22 @@
       <c r="F7" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="G7">
+        <f>CORREL($C$2:$C$11, A2:A11)</f>
+        <v>0.73719901064788396</v>
+      </c>
+      <c r="H7">
+        <f t="shared" ref="H7:J7" si="2">CORREL($C$2:$C$11, B2:B11)</f>
+        <v>-0.39911706248255019</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="2"/>
+        <v>-6.5867221172426202E-2</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -523,6 +577,22 @@
       </c>
       <c r="F8" s="2" t="s">
         <v>3</v>
+      </c>
+      <c r="G8">
+        <f>CORREL($D$2:$D$11, A2:A11)</f>
+        <v>0.48503173467607291</v>
+      </c>
+      <c r="H8">
+        <f t="shared" ref="H8:J8" si="3">CORREL($D$2:$D$11, B2:B11)</f>
+        <v>0.20257937544884455</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="3"/>
+        <v>-6.5867221172426202E-2</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>